<commit_message>
[FIX]pabi_budget_xls: fix for activity group list not coming in export costcontrol sheet ref:issues/1247#note-6
</commit_message>
<xml_diff>
--- a/pabi_budget_xls/template/Template_Section_Plan_17_nov.xlsx
+++ b/pabi_budget_xls/template/Template_Section_Plan_17_nov.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="716" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="716" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Section" sheetId="1" state="visible" r:id="rId2"/>
@@ -922,7 +922,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1560,8 +1560,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -11020,8 +11020,8 @@
   </sheetPr>
   <dimension ref="1:185"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y172" activeCellId="0" sqref="Y172"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E186" activeCellId="0" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -11363,7 +11363,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="45"/>
-      <c r="D14" s="50"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="50"/>
       <c r="F14" s="50"/>
       <c r="G14" s="50"/>
@@ -11405,7 +11405,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="45"/>
-      <c r="D15" s="50"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="50"/>
       <c r="F15" s="50"/>
       <c r="G15" s="50"/>
@@ -11447,7 +11447,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="45"/>
-      <c r="D16" s="50"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="50"/>
       <c r="F16" s="50"/>
       <c r="G16" s="50"/>
@@ -11489,7 +11489,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="45"/>
-      <c r="D17" s="50"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
       <c r="G17" s="50"/>
@@ -11531,7 +11531,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="45"/>
-      <c r="D18" s="50"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
       <c r="G18" s="50"/>
@@ -11573,7 +11573,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="45"/>
-      <c r="D19" s="50"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
       <c r="G19" s="50"/>
@@ -11615,7 +11615,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="45"/>
-      <c r="D20" s="50"/>
+      <c r="D20" s="46"/>
       <c r="E20" s="50"/>
       <c r="F20" s="50"/>
       <c r="G20" s="50"/>
@@ -11657,7 +11657,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="45"/>
-      <c r="D21" s="50"/>
+      <c r="D21" s="46"/>
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
       <c r="G21" s="50"/>
@@ -11699,7 +11699,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="45"/>
-      <c r="D22" s="50"/>
+      <c r="D22" s="46"/>
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -12021,7 +12021,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="45"/>
-      <c r="D31" s="37"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="47"/>
       <c r="F31" s="47"/>
       <c r="G31" s="47"/>
@@ -12064,7 +12064,7 @@
         <v>0</v>
       </c>
       <c r="C32" s="45"/>
-      <c r="D32" s="50"/>
+      <c r="D32" s="46"/>
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
       <c r="G32" s="50"/>
@@ -12106,7 +12106,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="45"/>
-      <c r="D33" s="50"/>
+      <c r="D33" s="46"/>
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
       <c r="G33" s="50"/>
@@ -12148,7 +12148,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="45"/>
-      <c r="D34" s="50"/>
+      <c r="D34" s="46"/>
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
       <c r="G34" s="50"/>
@@ -12190,7 +12190,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="45"/>
-      <c r="D35" s="50"/>
+      <c r="D35" s="46"/>
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
       <c r="G35" s="50"/>
@@ -12232,7 +12232,7 @@
         <v>0</v>
       </c>
       <c r="C36" s="45"/>
-      <c r="D36" s="50"/>
+      <c r="D36" s="46"/>
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
       <c r="G36" s="50"/>
@@ -12274,7 +12274,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="45"/>
-      <c r="D37" s="50"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="50"/>
       <c r="F37" s="50"/>
       <c r="G37" s="50"/>
@@ -12316,7 +12316,7 @@
         <v>0</v>
       </c>
       <c r="C38" s="45"/>
-      <c r="D38" s="50"/>
+      <c r="D38" s="46"/>
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
       <c r="G38" s="50"/>
@@ -12358,7 +12358,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="45"/>
-      <c r="D39" s="50"/>
+      <c r="D39" s="46"/>
       <c r="E39" s="50"/>
       <c r="F39" s="50"/>
       <c r="G39" s="50"/>
@@ -12400,7 +12400,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="45"/>
-      <c r="D40" s="50"/>
+      <c r="D40" s="46"/>
       <c r="E40" s="50"/>
       <c r="F40" s="50"/>
       <c r="G40" s="50"/>
@@ -12722,7 +12722,7 @@
         <v>0</v>
       </c>
       <c r="C49" s="45"/>
-      <c r="D49" s="37"/>
+      <c r="D49" s="46"/>
       <c r="E49" s="47"/>
       <c r="F49" s="47"/>
       <c r="G49" s="47"/>
@@ -12765,7 +12765,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="45"/>
-      <c r="D50" s="50"/>
+      <c r="D50" s="46"/>
       <c r="E50" s="50"/>
       <c r="F50" s="50"/>
       <c r="G50" s="50"/>
@@ -12807,7 +12807,7 @@
         <v>0</v>
       </c>
       <c r="C51" s="45"/>
-      <c r="D51" s="50"/>
+      <c r="D51" s="46"/>
       <c r="E51" s="50"/>
       <c r="F51" s="50"/>
       <c r="G51" s="50"/>
@@ -12849,7 +12849,7 @@
         <v>0</v>
       </c>
       <c r="C52" s="45"/>
-      <c r="D52" s="50"/>
+      <c r="D52" s="46"/>
       <c r="E52" s="50"/>
       <c r="F52" s="50"/>
       <c r="G52" s="50"/>
@@ -12891,7 +12891,7 @@
         <v>0</v>
       </c>
       <c r="C53" s="45"/>
-      <c r="D53" s="50"/>
+      <c r="D53" s="46"/>
       <c r="E53" s="50"/>
       <c r="F53" s="50"/>
       <c r="G53" s="50"/>
@@ -12933,7 +12933,7 @@
         <v>0</v>
       </c>
       <c r="C54" s="45"/>
-      <c r="D54" s="50"/>
+      <c r="D54" s="46"/>
       <c r="E54" s="50"/>
       <c r="F54" s="50"/>
       <c r="G54" s="50"/>
@@ -12975,7 +12975,7 @@
         <v>0</v>
       </c>
       <c r="C55" s="45"/>
-      <c r="D55" s="50"/>
+      <c r="D55" s="46"/>
       <c r="E55" s="50"/>
       <c r="F55" s="50"/>
       <c r="G55" s="50"/>
@@ -13017,7 +13017,7 @@
         <v>0</v>
       </c>
       <c r="C56" s="45"/>
-      <c r="D56" s="50"/>
+      <c r="D56" s="46"/>
       <c r="E56" s="50"/>
       <c r="F56" s="50"/>
       <c r="G56" s="50"/>
@@ -13059,7 +13059,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="45"/>
-      <c r="D57" s="50"/>
+      <c r="D57" s="46"/>
       <c r="E57" s="50"/>
       <c r="F57" s="50"/>
       <c r="G57" s="50"/>
@@ -13101,7 +13101,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="45"/>
-      <c r="D58" s="50"/>
+      <c r="D58" s="46"/>
       <c r="E58" s="50"/>
       <c r="F58" s="50"/>
       <c r="G58" s="50"/>
@@ -13423,7 +13423,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="45"/>
-      <c r="D67" s="37"/>
+      <c r="D67" s="46"/>
       <c r="E67" s="47"/>
       <c r="F67" s="47"/>
       <c r="G67" s="47"/>
@@ -13466,7 +13466,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="45"/>
-      <c r="D68" s="50"/>
+      <c r="D68" s="46"/>
       <c r="E68" s="50"/>
       <c r="F68" s="50"/>
       <c r="G68" s="50"/>
@@ -13508,7 +13508,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="45"/>
-      <c r="D69" s="50"/>
+      <c r="D69" s="46"/>
       <c r="E69" s="50"/>
       <c r="F69" s="50"/>
       <c r="G69" s="50"/>
@@ -13550,7 +13550,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="45"/>
-      <c r="D70" s="50"/>
+      <c r="D70" s="46"/>
       <c r="E70" s="50"/>
       <c r="F70" s="50"/>
       <c r="G70" s="50"/>
@@ -13592,7 +13592,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="45"/>
-      <c r="D71" s="50"/>
+      <c r="D71" s="46"/>
       <c r="E71" s="50"/>
       <c r="F71" s="50"/>
       <c r="G71" s="50"/>
@@ -13634,7 +13634,7 @@
         <v>0</v>
       </c>
       <c r="C72" s="45"/>
-      <c r="D72" s="50"/>
+      <c r="D72" s="46"/>
       <c r="E72" s="50"/>
       <c r="F72" s="50"/>
       <c r="G72" s="50"/>
@@ -13676,7 +13676,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="45"/>
-      <c r="D73" s="50"/>
+      <c r="D73" s="46"/>
       <c r="E73" s="50"/>
       <c r="F73" s="50"/>
       <c r="G73" s="50"/>
@@ -13718,7 +13718,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="45"/>
-      <c r="D74" s="50"/>
+      <c r="D74" s="46"/>
       <c r="E74" s="50"/>
       <c r="F74" s="50"/>
       <c r="G74" s="50"/>
@@ -13760,7 +13760,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="45"/>
-      <c r="D75" s="50"/>
+      <c r="D75" s="46"/>
       <c r="E75" s="50"/>
       <c r="F75" s="50"/>
       <c r="G75" s="50"/>
@@ -13802,7 +13802,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="45"/>
-      <c r="D76" s="50"/>
+      <c r="D76" s="46"/>
       <c r="E76" s="50"/>
       <c r="F76" s="50"/>
       <c r="G76" s="50"/>
@@ -14124,7 +14124,7 @@
         <v>0</v>
       </c>
       <c r="C85" s="45"/>
-      <c r="D85" s="37"/>
+      <c r="D85" s="46"/>
       <c r="E85" s="47"/>
       <c r="F85" s="47"/>
       <c r="G85" s="47"/>
@@ -14167,7 +14167,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="45"/>
-      <c r="D86" s="50"/>
+      <c r="D86" s="46"/>
       <c r="E86" s="50"/>
       <c r="F86" s="50"/>
       <c r="G86" s="50"/>
@@ -14209,7 +14209,7 @@
         <v>0</v>
       </c>
       <c r="C87" s="45"/>
-      <c r="D87" s="50"/>
+      <c r="D87" s="46"/>
       <c r="E87" s="50"/>
       <c r="F87" s="50"/>
       <c r="G87" s="50"/>
@@ -14251,7 +14251,7 @@
         <v>0</v>
       </c>
       <c r="C88" s="45"/>
-      <c r="D88" s="50"/>
+      <c r="D88" s="46"/>
       <c r="E88" s="50"/>
       <c r="F88" s="50"/>
       <c r="G88" s="50"/>
@@ -14293,7 +14293,7 @@
         <v>0</v>
       </c>
       <c r="C89" s="45"/>
-      <c r="D89" s="50"/>
+      <c r="D89" s="46"/>
       <c r="E89" s="50"/>
       <c r="F89" s="50"/>
       <c r="G89" s="50"/>
@@ -14335,7 +14335,7 @@
         <v>0</v>
       </c>
       <c r="C90" s="45"/>
-      <c r="D90" s="50"/>
+      <c r="D90" s="46"/>
       <c r="E90" s="50"/>
       <c r="F90" s="50"/>
       <c r="G90" s="50"/>
@@ -14377,7 +14377,7 @@
         <v>0</v>
       </c>
       <c r="C91" s="45"/>
-      <c r="D91" s="50"/>
+      <c r="D91" s="46"/>
       <c r="E91" s="50"/>
       <c r="F91" s="50"/>
       <c r="G91" s="50"/>
@@ -14419,7 +14419,7 @@
         <v>0</v>
       </c>
       <c r="C92" s="45"/>
-      <c r="D92" s="50"/>
+      <c r="D92" s="46"/>
       <c r="E92" s="50"/>
       <c r="F92" s="50"/>
       <c r="G92" s="50"/>
@@ -14461,7 +14461,7 @@
         <v>0</v>
       </c>
       <c r="C93" s="45"/>
-      <c r="D93" s="50"/>
+      <c r="D93" s="46"/>
       <c r="E93" s="50"/>
       <c r="F93" s="50"/>
       <c r="G93" s="50"/>
@@ -14503,7 +14503,7 @@
         <v>0</v>
       </c>
       <c r="C94" s="45"/>
-      <c r="D94" s="50"/>
+      <c r="D94" s="46"/>
       <c r="E94" s="50"/>
       <c r="F94" s="50"/>
       <c r="G94" s="50"/>
@@ -14825,7 +14825,7 @@
         <v>0</v>
       </c>
       <c r="C103" s="45"/>
-      <c r="D103" s="37"/>
+      <c r="D103" s="46"/>
       <c r="E103" s="47"/>
       <c r="F103" s="47"/>
       <c r="G103" s="47"/>
@@ -14868,7 +14868,7 @@
         <v>0</v>
       </c>
       <c r="C104" s="45"/>
-      <c r="D104" s="50"/>
+      <c r="D104" s="46"/>
       <c r="E104" s="50"/>
       <c r="F104" s="50"/>
       <c r="G104" s="50"/>
@@ -14910,7 +14910,7 @@
         <v>0</v>
       </c>
       <c r="C105" s="45"/>
-      <c r="D105" s="50"/>
+      <c r="D105" s="46"/>
       <c r="E105" s="50"/>
       <c r="F105" s="50"/>
       <c r="G105" s="50"/>
@@ -14952,7 +14952,7 @@
         <v>0</v>
       </c>
       <c r="C106" s="45"/>
-      <c r="D106" s="50"/>
+      <c r="D106" s="46"/>
       <c r="E106" s="50"/>
       <c r="F106" s="50"/>
       <c r="G106" s="50"/>
@@ -14994,7 +14994,7 @@
         <v>0</v>
       </c>
       <c r="C107" s="45"/>
-      <c r="D107" s="50"/>
+      <c r="D107" s="46"/>
       <c r="E107" s="50"/>
       <c r="F107" s="50"/>
       <c r="G107" s="50"/>
@@ -15036,7 +15036,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="45"/>
-      <c r="D108" s="50"/>
+      <c r="D108" s="46"/>
       <c r="E108" s="50"/>
       <c r="F108" s="50"/>
       <c r="G108" s="50"/>
@@ -15078,7 +15078,7 @@
         <v>0</v>
       </c>
       <c r="C109" s="45"/>
-      <c r="D109" s="50"/>
+      <c r="D109" s="46"/>
       <c r="E109" s="50"/>
       <c r="F109" s="50"/>
       <c r="G109" s="50"/>
@@ -15120,7 +15120,7 @@
         <v>0</v>
       </c>
       <c r="C110" s="45"/>
-      <c r="D110" s="50"/>
+      <c r="D110" s="46"/>
       <c r="E110" s="50"/>
       <c r="F110" s="50"/>
       <c r="G110" s="50"/>
@@ -15162,7 +15162,7 @@
         <v>0</v>
       </c>
       <c r="C111" s="45"/>
-      <c r="D111" s="50"/>
+      <c r="D111" s="46"/>
       <c r="E111" s="50"/>
       <c r="F111" s="50"/>
       <c r="G111" s="50"/>
@@ -15204,7 +15204,7 @@
         <v>0</v>
       </c>
       <c r="C112" s="45"/>
-      <c r="D112" s="50"/>
+      <c r="D112" s="46"/>
       <c r="E112" s="50"/>
       <c r="F112" s="50"/>
       <c r="G112" s="50"/>
@@ -15526,7 +15526,7 @@
         <v>0</v>
       </c>
       <c r="C121" s="45"/>
-      <c r="D121" s="37"/>
+      <c r="D121" s="46"/>
       <c r="E121" s="47"/>
       <c r="F121" s="47"/>
       <c r="G121" s="47"/>
@@ -15569,7 +15569,7 @@
         <v>0</v>
       </c>
       <c r="C122" s="45"/>
-      <c r="D122" s="50"/>
+      <c r="D122" s="46"/>
       <c r="E122" s="50"/>
       <c r="F122" s="50"/>
       <c r="G122" s="50"/>
@@ -15611,7 +15611,7 @@
         <v>0</v>
       </c>
       <c r="C123" s="45"/>
-      <c r="D123" s="50"/>
+      <c r="D123" s="46"/>
       <c r="E123" s="50"/>
       <c r="F123" s="50"/>
       <c r="G123" s="50"/>
@@ -15653,7 +15653,7 @@
         <v>0</v>
       </c>
       <c r="C124" s="45"/>
-      <c r="D124" s="50"/>
+      <c r="D124" s="46"/>
       <c r="E124" s="50"/>
       <c r="F124" s="50"/>
       <c r="G124" s="50"/>
@@ -15695,7 +15695,7 @@
         <v>0</v>
       </c>
       <c r="C125" s="45"/>
-      <c r="D125" s="50"/>
+      <c r="D125" s="46"/>
       <c r="E125" s="50"/>
       <c r="F125" s="50"/>
       <c r="G125" s="50"/>
@@ -15737,7 +15737,7 @@
         <v>0</v>
       </c>
       <c r="C126" s="45"/>
-      <c r="D126" s="50"/>
+      <c r="D126" s="46"/>
       <c r="E126" s="50"/>
       <c r="F126" s="50"/>
       <c r="G126" s="50"/>
@@ -15779,7 +15779,7 @@
         <v>0</v>
       </c>
       <c r="C127" s="45"/>
-      <c r="D127" s="50"/>
+      <c r="D127" s="46"/>
       <c r="E127" s="50"/>
       <c r="F127" s="50"/>
       <c r="G127" s="50"/>
@@ -15821,7 +15821,7 @@
         <v>0</v>
       </c>
       <c r="C128" s="45"/>
-      <c r="D128" s="50"/>
+      <c r="D128" s="46"/>
       <c r="E128" s="50"/>
       <c r="F128" s="50"/>
       <c r="G128" s="50"/>
@@ -15863,7 +15863,7 @@
         <v>0</v>
       </c>
       <c r="C129" s="45"/>
-      <c r="D129" s="50"/>
+      <c r="D129" s="46"/>
       <c r="E129" s="50"/>
       <c r="F129" s="50"/>
       <c r="G129" s="50"/>
@@ -15905,7 +15905,7 @@
         <v>0</v>
       </c>
       <c r="C130" s="45"/>
-      <c r="D130" s="50"/>
+      <c r="D130" s="46"/>
       <c r="E130" s="50"/>
       <c r="F130" s="50"/>
       <c r="G130" s="50"/>
@@ -16227,7 +16227,7 @@
         <v>0</v>
       </c>
       <c r="C139" s="45"/>
-      <c r="D139" s="37"/>
+      <c r="D139" s="46"/>
       <c r="E139" s="47"/>
       <c r="F139" s="47"/>
       <c r="G139" s="47"/>
@@ -16270,7 +16270,7 @@
         <v>0</v>
       </c>
       <c r="C140" s="45"/>
-      <c r="D140" s="50"/>
+      <c r="D140" s="46"/>
       <c r="E140" s="50"/>
       <c r="F140" s="50"/>
       <c r="G140" s="50"/>
@@ -16312,7 +16312,7 @@
         <v>0</v>
       </c>
       <c r="C141" s="45"/>
-      <c r="D141" s="50"/>
+      <c r="D141" s="46"/>
       <c r="E141" s="50"/>
       <c r="F141" s="50"/>
       <c r="G141" s="50"/>
@@ -16354,7 +16354,7 @@
         <v>0</v>
       </c>
       <c r="C142" s="45"/>
-      <c r="D142" s="50"/>
+      <c r="D142" s="46"/>
       <c r="E142" s="50"/>
       <c r="F142" s="50"/>
       <c r="G142" s="50"/>
@@ -16396,7 +16396,7 @@
         <v>0</v>
       </c>
       <c r="C143" s="45"/>
-      <c r="D143" s="50"/>
+      <c r="D143" s="46"/>
       <c r="E143" s="50"/>
       <c r="F143" s="50"/>
       <c r="G143" s="50"/>
@@ -16438,7 +16438,7 @@
         <v>0</v>
       </c>
       <c r="C144" s="45"/>
-      <c r="D144" s="50"/>
+      <c r="D144" s="46"/>
       <c r="E144" s="50"/>
       <c r="F144" s="50"/>
       <c r="G144" s="50"/>
@@ -16480,7 +16480,7 @@
         <v>0</v>
       </c>
       <c r="C145" s="45"/>
-      <c r="D145" s="50"/>
+      <c r="D145" s="46"/>
       <c r="E145" s="50"/>
       <c r="F145" s="50"/>
       <c r="G145" s="50"/>
@@ -16522,7 +16522,7 @@
         <v>0</v>
       </c>
       <c r="C146" s="45"/>
-      <c r="D146" s="50"/>
+      <c r="D146" s="46"/>
       <c r="E146" s="50"/>
       <c r="F146" s="50"/>
       <c r="G146" s="50"/>
@@ -16564,7 +16564,7 @@
         <v>0</v>
       </c>
       <c r="C147" s="45"/>
-      <c r="D147" s="50"/>
+      <c r="D147" s="46"/>
       <c r="E147" s="50"/>
       <c r="F147" s="50"/>
       <c r="G147" s="50"/>
@@ -16606,7 +16606,7 @@
         <v>0</v>
       </c>
       <c r="C148" s="45"/>
-      <c r="D148" s="50"/>
+      <c r="D148" s="46"/>
       <c r="E148" s="50"/>
       <c r="F148" s="50"/>
       <c r="G148" s="50"/>
@@ -16928,7 +16928,7 @@
         <v>0</v>
       </c>
       <c r="C157" s="45"/>
-      <c r="D157" s="37"/>
+      <c r="D157" s="46"/>
       <c r="E157" s="47"/>
       <c r="F157" s="47"/>
       <c r="G157" s="47"/>
@@ -16971,7 +16971,7 @@
         <v>0</v>
       </c>
       <c r="C158" s="45"/>
-      <c r="D158" s="50"/>
+      <c r="D158" s="46"/>
       <c r="E158" s="50"/>
       <c r="F158" s="50"/>
       <c r="G158" s="50"/>
@@ -17013,7 +17013,7 @@
         <v>0</v>
       </c>
       <c r="C159" s="45"/>
-      <c r="D159" s="50"/>
+      <c r="D159" s="46"/>
       <c r="E159" s="50"/>
       <c r="F159" s="50"/>
       <c r="G159" s="50"/>
@@ -17055,7 +17055,7 @@
         <v>0</v>
       </c>
       <c r="C160" s="45"/>
-      <c r="D160" s="50"/>
+      <c r="D160" s="46"/>
       <c r="E160" s="50"/>
       <c r="F160" s="50"/>
       <c r="G160" s="50"/>
@@ -17097,7 +17097,7 @@
         <v>0</v>
       </c>
       <c r="C161" s="45"/>
-      <c r="D161" s="50"/>
+      <c r="D161" s="46"/>
       <c r="E161" s="50"/>
       <c r="F161" s="50"/>
       <c r="G161" s="50"/>
@@ -17139,7 +17139,7 @@
         <v>0</v>
       </c>
       <c r="C162" s="45"/>
-      <c r="D162" s="50"/>
+      <c r="D162" s="46"/>
       <c r="E162" s="50"/>
       <c r="F162" s="50"/>
       <c r="G162" s="50"/>
@@ -17181,7 +17181,7 @@
         <v>0</v>
       </c>
       <c r="C163" s="45"/>
-      <c r="D163" s="50"/>
+      <c r="D163" s="46"/>
       <c r="E163" s="50"/>
       <c r="F163" s="50"/>
       <c r="G163" s="50"/>
@@ -17223,7 +17223,7 @@
         <v>0</v>
       </c>
       <c r="C164" s="45"/>
-      <c r="D164" s="50"/>
+      <c r="D164" s="46"/>
       <c r="E164" s="50"/>
       <c r="F164" s="50"/>
       <c r="G164" s="50"/>
@@ -17265,7 +17265,7 @@
         <v>0</v>
       </c>
       <c r="C165" s="45"/>
-      <c r="D165" s="50"/>
+      <c r="D165" s="46"/>
       <c r="E165" s="50"/>
       <c r="F165" s="50"/>
       <c r="G165" s="50"/>
@@ -17307,7 +17307,7 @@
         <v>0</v>
       </c>
       <c r="C166" s="45"/>
-      <c r="D166" s="50"/>
+      <c r="D166" s="46"/>
       <c r="E166" s="50"/>
       <c r="F166" s="50"/>
       <c r="G166" s="50"/>
@@ -17629,7 +17629,7 @@
         <v>0</v>
       </c>
       <c r="C175" s="45"/>
-      <c r="D175" s="37"/>
+      <c r="D175" s="46"/>
       <c r="E175" s="47"/>
       <c r="F175" s="47"/>
       <c r="G175" s="47"/>
@@ -17672,7 +17672,7 @@
         <v>0</v>
       </c>
       <c r="C176" s="45"/>
-      <c r="D176" s="50"/>
+      <c r="D176" s="46"/>
       <c r="E176" s="50"/>
       <c r="F176" s="50"/>
       <c r="G176" s="50"/>
@@ -17714,7 +17714,7 @@
         <v>0</v>
       </c>
       <c r="C177" s="45"/>
-      <c r="D177" s="50"/>
+      <c r="D177" s="46"/>
       <c r="E177" s="50"/>
       <c r="F177" s="50"/>
       <c r="G177" s="50"/>
@@ -17756,7 +17756,7 @@
         <v>0</v>
       </c>
       <c r="C178" s="45"/>
-      <c r="D178" s="50"/>
+      <c r="D178" s="46"/>
       <c r="E178" s="50"/>
       <c r="F178" s="50"/>
       <c r="G178" s="50"/>
@@ -17798,7 +17798,7 @@
         <v>0</v>
       </c>
       <c r="C179" s="45"/>
-      <c r="D179" s="50"/>
+      <c r="D179" s="46"/>
       <c r="E179" s="50"/>
       <c r="F179" s="50"/>
       <c r="G179" s="50"/>
@@ -17840,7 +17840,7 @@
         <v>0</v>
       </c>
       <c r="C180" s="45"/>
-      <c r="D180" s="50"/>
+      <c r="D180" s="46"/>
       <c r="E180" s="50"/>
       <c r="F180" s="50"/>
       <c r="G180" s="50"/>
@@ -17882,7 +17882,7 @@
         <v>0</v>
       </c>
       <c r="C181" s="45"/>
-      <c r="D181" s="50"/>
+      <c r="D181" s="46"/>
       <c r="E181" s="50"/>
       <c r="F181" s="50"/>
       <c r="G181" s="50"/>
@@ -17924,7 +17924,7 @@
         <v>0</v>
       </c>
       <c r="C182" s="45"/>
-      <c r="D182" s="50"/>
+      <c r="D182" s="46"/>
       <c r="E182" s="50"/>
       <c r="F182" s="50"/>
       <c r="G182" s="50"/>
@@ -17966,7 +17966,7 @@
         <v>0</v>
       </c>
       <c r="C183" s="45"/>
-      <c r="D183" s="50"/>
+      <c r="D183" s="46"/>
       <c r="E183" s="50"/>
       <c r="F183" s="50"/>
       <c r="G183" s="50"/>
@@ -18008,7 +18008,7 @@
         <v>0</v>
       </c>
       <c r="C184" s="45"/>
-      <c r="D184" s="50"/>
+      <c r="D184" s="46"/>
       <c r="E184" s="50"/>
       <c r="F184" s="50"/>
       <c r="G184" s="50"/>
@@ -18154,13 +18154,9 @@
     <mergeCell ref="G173:I173"/>
     <mergeCell ref="L173:X173"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B8 B26 B44 B62 B80 B98 B116 B134 B152 B170" type="list">
       <formula1>CostControl_MasterData!$C$2:$C$208</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D14:D22 D32:D40 D50:D58 D68:D76 D86:D94 D104:D112 D122:D130 D140:D148 D158:D166 D176:D184" type="list">
-      <formula1>#REF!!$C$2:$C$39</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FIX]pabi_budget_xls: changed p0-p12 as month name and now we will get excel output in xlsx format ref:issues/1285#note-2 , issues/1285#note-4
</commit_message>
<xml_diff>
--- a/pabi_budget_xls/template/Template_Section_Plan_17_nov.xlsx
+++ b/pabi_budget_xls/template/Template_Section_Plan_17_nov.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="716" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="716" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Section" sheetId="1" state="visible" r:id="rId2"/>
@@ -400,43 +400,43 @@
     <t>Budget</t>
   </si>
   <si>
-    <t>P0</t>
+    <t>&lt;</t>
   </si>
   <si>
-    <t>P1</t>
+    <t>Oct</t>
   </si>
   <si>
-    <t>P2</t>
+    <t>Nov</t>
   </si>
   <si>
-    <t>P3</t>
+    <t>Dec</t>
   </si>
   <si>
-    <t>P4</t>
+    <t>Jan</t>
   </si>
   <si>
-    <t>P5</t>
+    <t>Feb</t>
   </si>
   <si>
-    <t>P6</t>
+    <t>Mar</t>
   </si>
   <si>
-    <t>P7</t>
+    <t>Apr</t>
   </si>
   <si>
-    <t>P8</t>
+    <t>May</t>
   </si>
   <si>
-    <t>P9</t>
+    <t>Jun</t>
   </si>
   <si>
-    <t>P10</t>
+    <t>July</t>
   </si>
   <si>
-    <t>P11</t>
+    <t>Aug</t>
   </si>
   <si>
-    <t>P12</t>
+    <t>Sept</t>
   </si>
   <si>
     <t>Check</t>
@@ -995,7 +995,7 @@
   <dimension ref="A2:I56"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="1" sqref="H10:T10 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1498,7 +1498,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="H10:T10 A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1526,7 +1526,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="H10:T10 B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1554,8 +1554,8 @@
   </sheetPr>
   <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10:T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10976,8 +10976,8 @@
   </sheetPr>
   <dimension ref="1:185"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A172" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A189" activeCellId="0" sqref="A189"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G171" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H193" activeCellId="1" sqref="H10:T10 H193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>